<commit_message>
11-19 [Finish Ch1 ✨]
Alhumdulillah Finish chapter 1
</commit_message>
<xml_diff>
--- a/Word_AR.xlsx
+++ b/Word_AR.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Yaser Ammar\Documents\GitHub\Data_Science_BookTrip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507819A3-83C0-4884-B20D-782DDF55E1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28D6330-0D11-4C70-AB07-F1A120AC6AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="0" windowWidth="10000" windowHeight="12733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="132">
   <si>
     <t>word_EN</t>
   </si>
@@ -241,6 +244,186 @@
   </si>
   <si>
     <t>26-4-2023</t>
+  </si>
+  <si>
+    <t>despite</t>
+  </si>
+  <si>
+    <t>بالرغم من</t>
+  </si>
+  <si>
+    <t>acronym</t>
+  </si>
+  <si>
+    <t>اختصار</t>
+  </si>
+  <si>
+    <t>scares</t>
+  </si>
+  <si>
+    <t>يخيف</t>
+  </si>
+  <si>
+    <t>significance</t>
+  </si>
+  <si>
+    <t>دلالة</t>
+  </si>
+  <si>
+    <t>stochastic</t>
+  </si>
+  <si>
+    <t>العشوائية</t>
+  </si>
+  <si>
+    <t>instruct</t>
+  </si>
+  <si>
+    <t>إرشاد</t>
+  </si>
+  <si>
+    <t>fancy</t>
+  </si>
+  <si>
+    <t>خيالي؟</t>
+  </si>
+  <si>
+    <t>exhibited</t>
+  </si>
+  <si>
+    <t>عرضت</t>
+  </si>
+  <si>
+    <t>obstinacy</t>
+  </si>
+  <si>
+    <t>عناد</t>
+  </si>
+  <si>
+    <t>sympathize</t>
+  </si>
+  <si>
+    <t>تتعاطف</t>
+  </si>
+  <si>
+    <t>comprise</t>
+  </si>
+  <si>
+    <t>تضم</t>
+  </si>
+  <si>
+    <t>extent</t>
+  </si>
+  <si>
+    <t>مدى</t>
+  </si>
+  <si>
+    <t>expertise</t>
+  </si>
+  <si>
+    <t>خبرة</t>
+  </si>
+  <si>
+    <t>bolster</t>
+  </si>
+  <si>
+    <t>دعم</t>
+  </si>
+  <si>
+    <t>narrative</t>
+  </si>
+  <si>
+    <t>رواية</t>
+  </si>
+  <si>
+    <t>sophisticated</t>
+  </si>
+  <si>
+    <t>متطور</t>
+  </si>
+  <si>
+    <t>disempowering</t>
+  </si>
+  <si>
+    <t>إضعاف</t>
+  </si>
+  <si>
+    <t>meticulous</t>
+  </si>
+  <si>
+    <t>شديد الإنتباه للتفاصيل</t>
+  </si>
+  <si>
+    <t>groundbreaking</t>
+  </si>
+  <si>
+    <t>رائدة</t>
+  </si>
+  <si>
+    <t>unparalleled</t>
+  </si>
+  <si>
+    <t>لا مثيل لها</t>
+  </si>
+  <si>
+    <t>inquisitiveness</t>
+  </si>
+  <si>
+    <t>الفضول</t>
+  </si>
+  <si>
+    <t>messy data</t>
+  </si>
+  <si>
+    <t>بيانات فوضوية</t>
+  </si>
+  <si>
+    <t>sheer perseverance</t>
+  </si>
+  <si>
+    <t>المثابرة المطلقة</t>
+  </si>
+  <si>
+    <t>gravitate</t>
+  </si>
+  <si>
+    <t>تنجذب</t>
+  </si>
+  <si>
+    <t>gifted</t>
+  </si>
+  <si>
+    <t>موهوبين</t>
+  </si>
+  <si>
+    <t>savvy</t>
+  </si>
+  <si>
+    <t>الدهاء</t>
+  </si>
+  <si>
+    <t>acumen</t>
+  </si>
+  <si>
+    <t>الفطنة</t>
+  </si>
+  <si>
+    <t>evolved</t>
+  </si>
+  <si>
+    <t>تطورت</t>
+  </si>
+  <si>
+    <t>entrepreneur</t>
+  </si>
+  <si>
+    <t>رائد أعمال</t>
+  </si>
+  <si>
+    <t>risk-tolerant</t>
+  </si>
+  <si>
+    <t>متسامح مع المخاطر</t>
   </si>
 </sst>
 </file>
@@ -558,16 +741,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="16.703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.17578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
@@ -864,6 +1047,9 @@
       <c r="B26" t="s">
         <v>56</v>
       </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
@@ -872,6 +1058,9 @@
       <c r="B27" t="s">
         <v>58</v>
       </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
@@ -880,6 +1069,9 @@
       <c r="B28" t="s">
         <v>60</v>
       </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
@@ -888,6 +1080,9 @@
       <c r="B29" t="s">
         <v>61</v>
       </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
@@ -896,6 +1091,9 @@
       <c r="B30" t="s">
         <v>63</v>
       </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
@@ -904,6 +1102,9 @@
       <c r="B31" t="s">
         <v>66</v>
       </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
@@ -923,8 +1124,17 @@
       <c r="B33" t="s">
         <v>70</v>
       </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
       <c r="C34">
         <v>11</v>
       </c>
@@ -932,7 +1142,346 @@
         <v>71</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A56" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A59" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A63" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C65">
+        <v>19</v>
+      </c>
+      <c r="D65" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
32-35 [Finish Ch1] 🧩
Edit for before finish introduction only
</commit_message>
<xml_diff>
--- a/Word_AR.xlsx
+++ b/Word_AR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Yaser Ammar\Documents\GitHub\Data_Science_BookTrip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B40391-ECA5-48FD-8A5F-EBCBCE78B4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259E3A68-5D33-4348-AACD-1B4551F28CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="0" windowWidth="10000" windowHeight="12733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="181">
   <si>
     <t>word_EN</t>
   </si>
@@ -535,6 +535,42 @@
   </si>
   <si>
     <t>29-4-2023</t>
+  </si>
+  <si>
+    <t>cut-and-dried</t>
+  </si>
+  <si>
+    <t>قص و تجفيف</t>
+  </si>
+  <si>
+    <t>reminiscing</t>
+  </si>
+  <si>
+    <t>ذكريات</t>
+  </si>
+  <si>
+    <t>mendous storage</t>
+  </si>
+  <si>
+    <t>تخزين هائل</t>
+  </si>
+  <si>
+    <t>consequently</t>
+  </si>
+  <si>
+    <t>بناء على ذلك</t>
+  </si>
+  <si>
+    <t>fraud detection</t>
+  </si>
+  <si>
+    <t>الكشف عن الغش</t>
+  </si>
+  <si>
+    <t>broken up</t>
+  </si>
+  <si>
+    <t>إنفصلنا</t>
   </si>
 </sst>
 </file>
@@ -852,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1777,11 +1813,72 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A82" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" t="s">
+        <v>170</v>
+      </c>
       <c r="C82">
         <v>32</v>
       </c>
       <c r="D82" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A83" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" t="s">
+        <v>172</v>
+      </c>
+      <c r="C83">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A84" t="s">
+        <v>173</v>
+      </c>
+      <c r="B84" t="s">
+        <v>174</v>
+      </c>
+      <c r="C84">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A85" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" t="s">
+        <v>176</v>
+      </c>
+      <c r="C85">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A86" t="s">
+        <v>179</v>
+      </c>
+      <c r="B86" t="s">
+        <v>180</v>
+      </c>
+      <c r="C86">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A87" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
42-43 📜 No 👓
No glasses today but at least one page 👓
</commit_message>
<xml_diff>
--- a/Word_AR.xlsx
+++ b/Word_AR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Yaser Ammar\Documents\GitHub\Data_Science_BookTrip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F531F38-6179-4FEB-8AA1-872FEC738D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD68E1C-C404-4DF7-B4D8-CEF34BE029C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10000" yWindow="0" windowWidth="10000" windowHeight="12733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="185">
   <si>
     <t>word_EN</t>
   </si>
@@ -580,6 +580,9 @@
   </si>
   <si>
     <t>30-4-2023</t>
+  </si>
+  <si>
+    <t>1-5-2023</t>
   </si>
 </sst>
 </file>
@@ -897,7 +900,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
       <selection activeCell="A89" sqref="A89"/>
@@ -1904,6 +1907,11 @@
         <v>183</v>
       </c>
     </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="D89" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
43-51 [Finish Ch3 ✨]
Need review to this chapter and write notes 📝
</commit_message>
<xml_diff>
--- a/Word_AR.xlsx
+++ b/Word_AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Yaser Ammar\Documents\GitHub\Data_Science_BookTrip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD68E1C-C404-4DF7-B4D8-CEF34BE029C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B57628-76EA-485F-BADD-CC3D106B9716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10000" yWindow="0" windowWidth="10000" windowHeight="12733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
   <si>
     <t>word_EN</t>
   </si>
@@ -582,7 +582,19 @@
     <t>30-4-2023</t>
   </si>
   <si>
-    <t>1-5-2023</t>
+    <t>3-5-2023</t>
+  </si>
+  <si>
+    <t>reinforcement</t>
+  </si>
+  <si>
+    <t>تعزيز</t>
+  </si>
+  <si>
+    <t>embodied</t>
+  </si>
+  <si>
+    <t>متجسد</t>
   </si>
 </sst>
 </file>
@@ -900,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1908,8 +1920,28 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A89" t="s">
+        <v>185</v>
+      </c>
+      <c r="B89" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89">
+        <v>43</v>
+      </c>
       <c r="D89" t="s">
         <v>184</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A90" t="s">
+        <v>187</v>
+      </c>
+      <c r="B90" t="s">
+        <v>188</v>
+      </c>
+      <c r="C90">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
51-55 [ Math start ➕➖➗]
Start chapter of math fields
</commit_message>
<xml_diff>
--- a/Word_AR.xlsx
+++ b/Word_AR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Yaser Ammar\Documents\GitHub\Data_Science_BookTrip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B57628-76EA-485F-BADD-CC3D106B9716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DEDA07-C70E-43FC-B063-C9DD966B08C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="0" windowWidth="10000" windowHeight="12733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="198">
   <si>
     <t>word_EN</t>
   </si>
@@ -595,16 +595,49 @@
   </si>
   <si>
     <t>متجسد</t>
+  </si>
+  <si>
+    <t>alarmed over</t>
+  </si>
+  <si>
+    <t>بقلق أكثر</t>
+  </si>
+  <si>
+    <t>5-5-2023</t>
+  </si>
+  <si>
+    <t>firm grasp</t>
+  </si>
+  <si>
+    <t>قبضة قوية</t>
+  </si>
+  <si>
+    <t>entirety</t>
+  </si>
+  <si>
+    <t>مجمل</t>
+  </si>
+  <si>
+    <t>likelihood</t>
+  </si>
+  <si>
+    <t>احتمالية</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -912,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1944,8 +1977,56 @@
         <v>43</v>
       </c>
     </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A91" t="s">
+        <v>189</v>
+      </c>
+      <c r="B91" t="s">
+        <v>190</v>
+      </c>
+      <c r="C91">
+        <v>51</v>
+      </c>
+      <c r="D91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A92" t="s">
+        <v>192</v>
+      </c>
+      <c r="B92" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A93" t="s">
+        <v>194</v>
+      </c>
+      <c r="B93" t="s">
+        <v>195</v>
+      </c>
+      <c r="C93">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A94" t="s">
+        <v>196</v>
+      </c>
+      <c r="B94" t="s">
+        <v>197</v>
+      </c>
+      <c r="C94">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>